<commit_message>
login page changes (Added Verification code)
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00FEBC2-14BC-4B1D-82FF-0BE61BA676BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B7A77D03-CB3B-40BF-B8D2-B8F275C279D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12" yWindow="0" windowWidth="23016" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>er.ashishcoer+11@gmail.com</t>
   </si>
@@ -32,6 +33,15 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Verification code</t>
+  </si>
+  <si>
+    <t>viswanath.aiyer@westernunion.com.uatcomm</t>
+  </si>
+  <si>
+    <t>Tulip@9211</t>
   </si>
 </sst>
 </file>
@@ -82,10 +92,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -367,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,26 +392,46 @@
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
+      </c>
+      <c r="C2">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>12345678</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E0829920-C206-4049-98C9-60B1ED8FFDE0}"/>
+    <hyperlink ref="A3" r:id="rId2" display="mailto:viswanath.aiyer@westernunion.com.uatcomm" xr:uid="{6DA98CD3-966F-4F46-B39A-7504B33C0881}"/>
+    <hyperlink ref="B3" r:id="rId3" display="mailto:Tulip@9211" xr:uid="{D8235375-54E3-48CB-A828-231E0532289F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>